<commit_message>
Updated Card Stats Added New Cards
</commit_message>
<xml_diff>
--- a/data/card_stats/card_stats.xlsx
+++ b/data/card_stats/card_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200142\Documents\Year 12\Card-Game\data\card_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5EB87A-6F0E-4764-98AA-CB45AFDE845C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EA4589-1048-4077-8CAE-A8EB32C54D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -120,21 +120,12 @@
     <t>Iteration 2 of Card Design</t>
   </si>
   <si>
-    <t>Drain</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Gain 2hp</t>
-  </si>
-  <si>
     <t>Slash</t>
   </si>
   <si>
-    <t>Hit all enemys for 6 damage</t>
-  </si>
-  <si>
     <t>Belly Drum</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
     <t xml:space="preserve">Swords Stance </t>
   </si>
   <si>
-    <t>Gives the player 3 Stab Cards</t>
-  </si>
-  <si>
     <t>Stab</t>
   </si>
   <si>
@@ -306,15 +294,9 @@
     <t>Health Drain</t>
   </si>
   <si>
-    <t>Deal 4 damage to the player but give 4 strength for the rest of combat</t>
-  </si>
-  <si>
     <t>Mega Bulk</t>
   </si>
   <si>
-    <t>Directly gives the player 5 Block, 50% of Block carrys over to next turn</t>
-  </si>
-  <si>
     <t>Directly gives the player 5 Block</t>
   </si>
   <si>
@@ -330,15 +312,9 @@
     <t>Acidic Touch</t>
   </si>
   <si>
-    <t>Whenever you attack an enemy, inflict 1 poison</t>
-  </si>
-  <si>
     <t>Prankster</t>
   </si>
   <si>
-    <t>Inflicts confusion on the enemy</t>
-  </si>
-  <si>
     <t>Confusion (Enemy)</t>
   </si>
   <si>
@@ -357,19 +333,88 @@
     <t>Handyman</t>
   </si>
   <si>
-    <t>The player keeps 2 cards in their hand at the end of the turn</t>
-  </si>
-  <si>
-    <t>See the enemy's intensions for the next 3 turns</t>
-  </si>
-  <si>
     <t>Last Resort</t>
   </si>
   <si>
-    <t>Gives the player 99 Block. Block can't be gained for the next 2 turns.</t>
-  </si>
-  <si>
     <t>If the player takes unblocked damage, heal for X hp</t>
+  </si>
+  <si>
+    <t>Vampirism</t>
+  </si>
+  <si>
+    <t>Final Blow</t>
+  </si>
+  <si>
+    <t>If this attack is not Fatal, die.</t>
+  </si>
+  <si>
+    <t>Wire Transfer</t>
+  </si>
+  <si>
+    <t>Swaps all of your status conditions with an enemy</t>
+  </si>
+  <si>
+    <t>Gain 5 Block for the next 2 turns</t>
+  </si>
+  <si>
+    <t>Inflict 1 poison whenever you attack on the enemy you hit</t>
+  </si>
+  <si>
+    <t>Confuses the enemy</t>
+  </si>
+  <si>
+    <t>See enemy intensions for the next 3 turns. Foresight</t>
+  </si>
+  <si>
+    <t>Foresight</t>
+  </si>
+  <si>
+    <t>See enemy intentions for the next X turns</t>
+  </si>
+  <si>
+    <t>Keep 2 cards in the players hand at the end of the turn</t>
+  </si>
+  <si>
+    <t>Gain 99 Block. Block can't be gained for the next 2 turns.</t>
+  </si>
+  <si>
+    <t>Drain Punch</t>
+  </si>
+  <si>
+    <t>Wild Strike</t>
+  </si>
+  <si>
+    <t>Deal 30 damage. Cost decreases by 1 mana everytime played</t>
+  </si>
+  <si>
+    <t>Loose 4HP, +4 strength for the rest of combat</t>
+  </si>
+  <si>
+    <t>Deal 3 damage. Gain 2hp</t>
+  </si>
+  <si>
+    <t>Hit all enemys for 7 damage</t>
+  </si>
+  <si>
+    <t>Gives the player 4 Stab Cards, gain 1 strength</t>
+  </si>
+  <si>
+    <t>Sacrificial Power</t>
+  </si>
+  <si>
+    <t>Loose 4HP, +2 mana next turn</t>
+  </si>
+  <si>
+    <t>Sacred Sword</t>
+  </si>
+  <si>
+    <t>Double strength</t>
+  </si>
+  <si>
+    <t>Double block</t>
+  </si>
+  <si>
+    <t>Thick Fat</t>
   </si>
 </sst>
 </file>
@@ -695,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,7 +856,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -857,7 +902,7 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -890,224 +935,287 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18">
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E31" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33">
+        <v>25</v>
+      </c>
+      <c r="E33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36">
+        <v>-4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53" t="s">
+        <v>50</v>
+      </c>
+      <c r="F53" t="s">
         <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" t="s">
-        <v>54</v>
-      </c>
-      <c r="F53" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F54">
         <v>5</v>
@@ -1115,58 +1223,58 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>10</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D55" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>20</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D56" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D57" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B58">
         <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D58" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F58">
         <v>5</v>
@@ -1174,31 +1282,31 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E62" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E63" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E64" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.3">
@@ -1206,23 +1314,23 @@
         <v>10</v>
       </c>
       <c r="E65" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E66" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E67" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="4:5" x14ac:dyDescent="0.3">
@@ -1230,43 +1338,54 @@
         <v>20</v>
       </c>
       <c r="E68" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E69" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E70" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D71" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E71" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D72" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E72" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>101</v>
+      </c>
       <c r="E73" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D74" t="s">
+        <v>110</v>
+      </c>
+      <c r="E74" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1279,6 +1398,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A463F7EE9421341AB859790BF63E6BD" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9508db64953a7b123011b0874d62a3fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f3acae90-a355-41d8-8d71-6861ca761c67" xmlns:ns4="de5b240f-e61b-47c3-951f-24adcaf6e800" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bce019156a9591e0a8c154b9da1d2e4" ns3:_="" ns4:_="">
     <xsd:import namespace="f3acae90-a355-41d8-8d71-6861ca761c67"/>
@@ -1513,12 +1638,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1529,6 +1648,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC51933-8D9F-4635-A308-2890C5F65DC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E4F101-6772-41A1-81E0-8BD524C284D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1547,15 +1675,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC51933-8D9F-4635-A308-2890C5F65DC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7E5954-CA29-47CE-970F-5EF101E37214}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Coding in effects both the player and enemy can have.
</commit_message>
<xml_diff>
--- a/data/card_stats/card_stats.xlsx
+++ b/data/card_stats/card_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200142\Documents\Year 12\Card-Game\data\card_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EA4589-1048-4077-8CAE-A8EB32C54D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411D7B52-0402-4B15-ADC5-3DD4112E7D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1398,12 +1398,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A463F7EE9421341AB859790BF63E6BD" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9508db64953a7b123011b0874d62a3fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f3acae90-a355-41d8-8d71-6861ca761c67" xmlns:ns4="de5b240f-e61b-47c3-951f-24adcaf6e800" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bce019156a9591e0a8c154b9da1d2e4" ns3:_="" ns4:_="">
     <xsd:import namespace="f3acae90-a355-41d8-8d71-6861ca761c67"/>
@@ -1638,6 +1632,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1648,15 +1648,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC51933-8D9F-4635-A308-2890C5F65DC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E4F101-6772-41A1-81E0-8BD524C284D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1675,6 +1666,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC51933-8D9F-4635-A308-2890C5F65DC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7E5954-CA29-47CE-970F-5EF101E37214}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Coding more effects that can be applied to both enemies and player.
</commit_message>
<xml_diff>
--- a/data/card_stats/card_stats.xlsx
+++ b/data/card_stats/card_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200142\Documents\Year 12\Card-Game\data\card_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411D7B52-0402-4B15-ADC5-3DD4112E7D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1913072-E8D2-4610-94D1-D347AE45551A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -742,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -1398,6 +1398,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A463F7EE9421341AB859790BF63E6BD" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9508db64953a7b123011b0874d62a3fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f3acae90-a355-41d8-8d71-6861ca761c67" xmlns:ns4="de5b240f-e61b-47c3-951f-24adcaf6e800" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bce019156a9591e0a8c154b9da1d2e4" ns3:_="" ns4:_="">
     <xsd:import namespace="f3acae90-a355-41d8-8d71-6861ca761c67"/>
@@ -1632,12 +1638,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1648,6 +1648,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC51933-8D9F-4635-A308-2890C5F65DC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E4F101-6772-41A1-81E0-8BD524C284D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1666,15 +1675,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC51933-8D9F-4635-A308-2890C5F65DC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7E5954-CA29-47CE-970F-5EF101E37214}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed card replacement and removing of card slots, fixed effects,
</commit_message>
<xml_diff>
--- a/data/card_stats/card_stats.xlsx
+++ b/data/card_stats/card_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200142\Documents\Year 12\Card-Game\data\card_stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200107\Downloads\Python\Projects\Card Game\data\card_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1913072-E8D2-4610-94D1-D347AE45551A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8084D5C-0526-41A5-9470-3C3FE5F7E1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Attack</t>
   </si>
   <si>
-    <t>HP/Defence</t>
-  </si>
-  <si>
     <t>Effect</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>A Thousand Cuts</t>
   </si>
   <si>
-    <t>5 to 20</t>
-  </si>
-  <si>
     <t>Damage the enemy anywhere from 1-4 times dealing 5 damage per attack</t>
   </si>
   <si>
@@ -99,18 +93,12 @@
     <t>Health Pool</t>
   </si>
   <si>
-    <t>5hp</t>
-  </si>
-  <si>
     <t>Directly heals the player for 5 health if no shields are up</t>
   </si>
   <si>
     <t>Bulk Up</t>
   </si>
   <si>
-    <t>5def</t>
-  </si>
-  <si>
     <t>Punch</t>
   </si>
   <si>
@@ -415,13 +403,22 @@
   </si>
   <si>
     <t>Thick Fat</t>
+  </si>
+  <si>
+    <t>Defence/HP</t>
+  </si>
+  <si>
+    <t>5/0</t>
+  </si>
+  <si>
+    <t>0/0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +431,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -456,10 +459,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,26 +771,26 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -793,70 +798,70 @@
       <c r="C3">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -864,50 +869,50 @@
       <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
+      <c r="D7" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -915,14 +920,14 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
-        <v>9</v>
+      <c r="D10" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -930,225 +935,225 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C25">
         <v>-5</v>
       </c>
       <c r="E25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E32" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C33">
         <v>25</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -1157,65 +1162,65 @@
         <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C36">
         <v>-4</v>
       </c>
       <c r="E36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E37" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E38" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" t="s">
         <v>47</v>
-      </c>
-      <c r="B53" t="s">
-        <v>48</v>
-      </c>
-      <c r="C53" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" t="s">
-        <v>50</v>
-      </c>
-      <c r="F53" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B54">
         <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F54">
         <v>5</v>
@@ -1223,58 +1228,58 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B55">
         <v>10</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>20</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B58">
         <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D58" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F58">
         <v>5</v>
@@ -1282,128 +1287,123 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E62" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E63" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E64" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E65" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E66" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E67" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E68" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E69" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E70" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D71" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E71" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D72" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E72" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E73" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E74" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:G9 A10:F10" xr:uid="{8800CCAD-0168-47BA-A161-0D792C9EC343}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:F10 A1:G9" xr:uid="{8800CCAD-0168-47BA-A161-0D792C9EC343}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A463F7EE9421341AB859790BF63E6BD" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9508db64953a7b123011b0874d62a3fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f3acae90-a355-41d8-8d71-6861ca761c67" xmlns:ns4="de5b240f-e61b-47c3-951f-24adcaf6e800" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bce019156a9591e0a8c154b9da1d2e4" ns3:_="" ns4:_="">
     <xsd:import namespace="f3acae90-a355-41d8-8d71-6861ca761c67"/>
@@ -1638,6 +1638,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1648,15 +1654,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC51933-8D9F-4635-A308-2890C5F65DC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E4F101-6772-41A1-81E0-8BD524C284D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1675,6 +1672,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC51933-8D9F-4635-A308-2890C5F65DC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7E5954-CA29-47CE-970F-5EF101E37214}">
   <ds:schemaRefs>

</xml_diff>